<commit_message>
Last Sync: 2021-04-06 10:30:02
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -14,39 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
-  <si>
-    <t>SOW - Client</t>
-  </si>
-  <si>
-    <t>MSA - Vendor</t>
-  </si>
-  <si>
-    <t>Miscellaneous - Vendor</t>
-  </si>
-  <si>
-    <t>NDA - Client</t>
-  </si>
-  <si>
-    <t>Miscellaneous - Client</t>
-  </si>
-  <si>
-    <t>MSA - Client</t>
-  </si>
-  <si>
-    <t>BAA - Client</t>
-  </si>
-  <si>
-    <t>PSA - Vendor</t>
-  </si>
-  <si>
-    <t>PSA - Client</t>
-  </si>
-  <si>
-    <t>DPA - Client</t>
-  </si>
-  <si>
-    <t>NDA - Vendor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="28">
+  <si>
+    <t>SOW</t>
+  </si>
+  <si>
+    <t>MSA</t>
+  </si>
+  <si>
+    <t>Hubspot legal terms &amp; conditions</t>
+  </si>
+  <si>
+    <t>NDA</t>
+  </si>
+  <si>
+    <t>Code of Conduct</t>
+  </si>
+  <si>
+    <t>BAA</t>
+  </si>
+  <si>
+    <t>PSA</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Order Form</t>
+  </si>
+  <si>
+    <t>DPA</t>
+  </si>
+  <si>
+    <t>SDPA</t>
+  </si>
+  <si>
+    <t>Partner Affiliate Adoption Agreement</t>
+  </si>
+  <si>
+    <t>Referral Agreement</t>
+  </si>
+  <si>
+    <t>Engagement Letter</t>
   </si>
   <si>
     <t>Q-Tempelate</t>
@@ -58,7 +67,37 @@
     <t>Not enough data</t>
   </si>
   <si>
-    <t>SOW - Vendor</t>
+    <t>ZoomInfo Recurring credits</t>
+  </si>
+  <si>
+    <t>Change Order</t>
+  </si>
+  <si>
+    <t>Purchase Order</t>
+  </si>
+  <si>
+    <t>Lease Agreement</t>
+  </si>
+  <si>
+    <t>software license agreement</t>
+  </si>
+  <si>
+    <t>POC</t>
+  </si>
+  <si>
+    <t>Sponsorship Agreement</t>
+  </si>
+  <si>
+    <t>Partner Affliate Consent Letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSA </t>
+  </si>
+  <si>
+    <t>Addendum</t>
+  </si>
+  <si>
+    <t>Partner Agreement</t>
   </si>
 </sst>
 </file>
@@ -416,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,183 +495,264 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1.125</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="C2">
+        <v>4.466666666666667</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>5.272727272727272</v>
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>2.5</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>3.125</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>0.6</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
-        <v>3.25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>2.333333333333333</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:17">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>1</v>
+      <c r="B8">
+        <v>1.285714285714286</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>1.5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>1.909090909090909</v>
-      </c>
-      <c r="C9">
-        <v>2.375</v>
+        <v>1.75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>1.733333333333333</v>
+        <v>1.818181818181818</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>